<commit_message>
after updating pre-post cor after inclusing one more study
</commit_message>
<xml_diff>
--- a/Data/pre_post_correlations.xlsx
+++ b/Data/pre_post_correlations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Author</t>
   </si>
@@ -36,6 +36,15 @@
   </si>
   <si>
     <t xml:space="preserve">Shapira et al. (2007)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karkosz et al. (2024)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sun et al. (2023)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baez et al. (2017)</t>
   </si>
 </sst>
 </file>
@@ -433,6 +442,39 @@
         <v>0.805273356455184</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.803826184793257</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.973169571781571</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.0916082071125613</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.999916682001268</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.826887932363078</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.453098578130092</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
after incorporating data from more recent studies
</commit_message>
<xml_diff>
--- a/Data/pre_post_correlations.xlsx
+++ b/Data/pre_post_correlations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Author</t>
   </si>
@@ -41,7 +41,13 @@
     <t xml:space="preserve">Karkosz et al. (2024)</t>
   </si>
   <si>
-    <t xml:space="preserve">Sun et al. (2023)</t>
+    <t xml:space="preserve">Sun (2023)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brog et al. (2022)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iyer et al. (2023)</t>
   </si>
   <si>
     <t xml:space="preserve">Baez et al. (2017)</t>
@@ -469,9 +475,31 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
+        <v>0.137092597312419</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.994257446012105</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.0929704290319567</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.991422978792847</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="n">
         <v>0.826887932363078</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C11" t="n">
         <v>0.453098578130092</v>
       </c>
     </row>

</xml_diff>